<commit_message>
fix (dicionario de dados) - alterados os valores dos campos
</commit_message>
<xml_diff>
--- a/trabalho parte 1/Dicionario_de_Dados.xlsx
+++ b/trabalho parte 1/Dicionario_de_Dados.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
   <si>
     <t>Nome da tabela: alunos</t>
   </si>
@@ -46,9 +46,6 @@
     <t>nome</t>
   </si>
   <si>
-    <t>NOT NULL</t>
-  </si>
-  <si>
     <t>nome do aluno</t>
   </si>
   <si>
@@ -67,7 +64,7 @@
     <t>data_nasc</t>
   </si>
   <si>
-    <t>data</t>
+    <t>datetime</t>
   </si>
   <si>
     <t>data_nasc do aluno</t>
@@ -103,6 +100,9 @@
     <t>id_treino</t>
   </si>
   <si>
+    <t>bigint</t>
+  </si>
+  <si>
     <t>cod.identificação do Treino</t>
   </si>
   <si>
@@ -190,7 +190,7 @@
     <t>valor_pagamento</t>
   </si>
   <si>
-    <t>decimal</t>
+    <t>double</t>
   </si>
   <si>
     <t>Valor do pagamento</t>
@@ -221,21 +221,6 @@
   </si>
   <si>
     <t>Cod.Identificação do Treino</t>
-  </si>
-  <si>
-    <t>Nome da tabela: Aluno_Plano</t>
-  </si>
-  <si>
-    <t>Cod.Identificação do Plano</t>
-  </si>
-  <si>
-    <t>Nome da tabela: Pagar</t>
-  </si>
-  <si>
-    <t>Cod.identificação do plano</t>
-  </si>
-  <si>
-    <t>Cod.Identificação do Pagamento</t>
   </si>
   <si>
     <t>Nome da tabela: Instrutores_Treinos</t>
@@ -672,87 +657,77 @@
         <v>7</v>
       </c>
       <c r="C4" s="10">
-        <v>100.0</v>
-      </c>
-      <c r="D4" s="9" t="s">
+        <v>255.0</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7">
-        <v>50.0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="10">
+        <v>255.0</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="7">
-        <v>8.0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="H7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -760,33 +735,29 @@
       <c r="C9" s="7">
         <v>255.0</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="C10" s="7">
+        <v>255.0</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>7</v>
@@ -794,11 +765,9 @@
       <c r="C11" s="15">
         <v>255.0</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
@@ -817,7 +786,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -843,13 +812,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="C16" s="7">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>8</v>
@@ -866,11 +835,9 @@
         <v>7</v>
       </c>
       <c r="C17" s="10">
-        <v>100.0</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="11" t="s">
         <v>32</v>
       </c>
@@ -885,9 +852,7 @@
       <c r="C18" s="7">
         <v>255.0</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D18" s="6"/>
       <c r="E18" s="12" t="s">
         <v>34</v>
       </c>
@@ -900,11 +865,9 @@
         <v>36</v>
       </c>
       <c r="C19" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>11</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="D19" s="19"/>
       <c r="E19" s="21" t="s">
         <v>37</v>
       </c>
@@ -947,10 +910,10 @@
         <v>39</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>8</v>
@@ -967,86 +930,76 @@
         <v>7</v>
       </c>
       <c r="C24" s="10">
-        <v>100.0</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D24" s="9"/>
       <c r="E24" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="7">
-        <v>50.0</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C25" s="10">
+        <v>255.0</v>
+      </c>
+      <c r="D25" s="6"/>
       <c r="E25" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D26" s="9"/>
       <c r="E26" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C27" s="7">
-        <v>8.0</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>6.0</v>
+      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D28" s="9"/>
       <c r="E28" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>7</v>
@@ -1054,33 +1007,29 @@
       <c r="C29" s="7">
         <v>255.0</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D29" s="6"/>
       <c r="E29" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D30" s="9"/>
       <c r="E30" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>7</v>
@@ -1088,9 +1037,7 @@
       <c r="C31" s="23">
         <v>255.0</v>
       </c>
-      <c r="D31" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="D31" s="22"/>
       <c r="E31" s="24" t="s">
         <v>48</v>
       </c>
@@ -1105,9 +1052,7 @@
       <c r="C32" s="10">
         <v>255.0</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="D32" s="9"/>
       <c r="E32" s="11" t="s">
         <v>50</v>
       </c>
@@ -1122,9 +1067,7 @@
       <c r="C33" s="15">
         <v>255.0</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="D33" s="14"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -1167,10 +1110,10 @@
         <v>54</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C37" s="7">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>8</v>
@@ -1184,14 +1127,12 @@
         <v>56</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>6.0</v>
+      </c>
+      <c r="D38" s="9"/>
       <c r="E38" s="11" t="s">
         <v>57</v>
       </c>
@@ -1204,11 +1145,9 @@
         <v>59</v>
       </c>
       <c r="C39" s="7">
-        <v>7.0</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>8.0</v>
+      </c>
+      <c r="D39" s="6"/>
       <c r="E39" s="12" t="s">
         <v>60</v>
       </c>
@@ -1251,10 +1190,10 @@
         <v>62</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C43" s="7">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>8</v>
@@ -1271,11 +1210,9 @@
         <v>7</v>
       </c>
       <c r="C44" s="10">
-        <v>50.0</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>255.0</v>
+      </c>
+      <c r="D44" s="9"/>
       <c r="E44" s="11" t="s">
         <v>65</v>
       </c>
@@ -1290,9 +1227,7 @@
       <c r="C45" s="7">
         <v>255.0</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D45" s="6"/>
       <c r="E45" s="12" t="s">
         <v>66</v>
       </c>
@@ -1349,13 +1284,13 @@
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="C50" s="10">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>68</v>
@@ -1372,198 +1307,98 @@
       <c r="E51" s="18"/>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="3" t="s">
+    <row r="54">
+      <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C55" s="7">
         <v>11.0</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="D55" s="9" t="s">
+      <c r="E55" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="18"/>
-    </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E57" s="26"/>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59">
-      <c r="A59" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="7">
-        <v>11.0</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="E59" s="26"/>
     </row>
     <row r="60">
-      <c r="A60" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>74</v>
-      </c>
+      <c r="E60" s="26"/>
     </row>
     <row r="61">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="18"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E62" s="26"/>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="5"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64">
-      <c r="A64" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="7">
-        <v>11.0</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="E64" s="26"/>
     </row>
     <row r="65">
-      <c r="A65" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>76</v>
-      </c>
+      <c r="E65" s="26"/>
     </row>
     <row r="66">
       <c r="E66" s="26"/>
@@ -4345,33 +4180,6 @@
     </row>
     <row r="992">
       <c r="E992" s="26"/>
-    </row>
-    <row r="993">
-      <c r="E993" s="26"/>
-    </row>
-    <row r="994">
-      <c r="E994" s="26"/>
-    </row>
-    <row r="995">
-      <c r="E995" s="26"/>
-    </row>
-    <row r="996">
-      <c r="E996" s="26"/>
-    </row>
-    <row r="997">
-      <c r="E997" s="26"/>
-    </row>
-    <row r="998">
-      <c r="E998" s="26"/>
-    </row>
-    <row r="999">
-      <c r="E999" s="26"/>
-    </row>
-    <row r="1000">
-      <c r="E1000" s="26"/>
-    </row>
-    <row r="1001">
-      <c r="E1001" s="26"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>

</xml_diff>